<commit_message>
se realizan cambios en contenidoClasesNegocio codigo y excel
</commit_message>
<xml_diff>
--- a/docs/test-cases/contenidoClasesNegocio.xlsx
+++ b/docs/test-cases/contenidoClasesNegocio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
   <si>
     <t>ID Caso</t>
   </si>
@@ -117,15 +117,106 @@
     <t>Crear un modelo</t>
   </si>
   <si>
-    <t>Haber seleccionado la entidad modelos</t>
-  </si>
-  <si>
     <t>CP_CONCLNEG_004</t>
   </si>
   <si>
     <t>1.Clic en el botón "+" (Nuevo)
 2.Clic en botón del campo "Fabricante"
-3.Seleccionar fila del fabricante con ID "1" (HUAWEI)</t>
+3.Seleccionar fila del fabricante con ID "1" (HUAWEI)
+4.Clic en el botón "Seleccionar" tras elegir fabricante
+5.Diligenciar campo "Nombre" con "TEST CREAR"
+6.Diligenciar "Cantidad de slots" con número aleatorio
+7.Clic en el botón del campo "Tipo"
+8.Seleccionar tipo NOMBRE "ELEMENTO TERCIARIO - GADGETS" (fila ID 21)
+9.Clic en el botón "Seleccionar" del modal de tipo
+10.Diligenciar campo "Descripción"
+11.Diligenciar campo "Ícono"
+12.Clic en el botón del campo "Localidad"
+13.Clic en botón "Seleccionar" del modal de Localidad
+14.Clic en el botón "Guardar"</t>
+  </si>
+  <si>
+    <t>Editar modelo</t>
+  </si>
+  <si>
+    <t>Haber seleccionado la entidad modelos ocpion crear</t>
+  </si>
+  <si>
+    <t>Haber seleccionado la entidad modelos opcion editar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en el botón de la tabla (picklist)
+2.Seleccionar la entidad con ALIAS "Modelos"
+3.Clic en el botón "Seleccionar"
+4.Clic en botón Editar.
+5.Clic en el botón del campo "Fabricante" (modo edición)
+6.Seleccionar fabricante con ID 2 (FIBERHOME)
+7.Clic en botón "Seleccionar" del modal Fabricante
+8.Editar campo "Nombre" con "TEST EDITAR"
+9.Editar campo "Cantidad de slots" con valor aleatorio 51–100
+10.Clic en botón "Tipo"
+11.Seleccionar fila con ID 1 (ELEMENTO PRIMARIO - ACCESO)
+12.Clic en "Seleccionar" del modal Tipo
+13.Editar campo "Descripción"
+14.Clic en botón "Guardar" (formulario edición)
+</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_005</t>
+  </si>
+  <si>
+    <t>Haber seleccionado la entidad modelos opcion eliminar</t>
+  </si>
+  <si>
+    <t>1.Buscar el modelo "TEST EDITAR"
+2.Seleccionar registro con mayor ID
+3.Clic en botón "Eliminar"
+4.Confirmar eliminación en modal.</t>
+  </si>
+  <si>
+    <t>Eliminar modelo</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_006</t>
+  </si>
+  <si>
+    <t>Refrescar vista</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(modelo).</t>
+  </si>
+  <si>
+    <t>1.Clic en el boton refrescar</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_007</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado el botón generar reporte xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
+2.Clic en opción 'Exportar todos los registros'
+</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_008</t>
+  </si>
+  <si>
+    <t>Generar reporte xls (opcion exportar todos los registros)</t>
+  </si>
+  <si>
+    <t>Validar funcionamiento del paginador en la vista(Entidad planes comerciales)</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(planes comerciales).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
+2.Seleccionar la entidad con ID 135 ("Valores de planes")
+3.Clic en botón "Seleccionar"
+4.Clic en botón "Página siguiente"
+</t>
   </si>
 </sst>
 </file>
@@ -533,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -652,12 +743,8 @@
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
         <v>16</v>
       </c>
@@ -682,20 +769,16 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>16</v>
       </c>
@@ -708,10 +791,10 @@
     </row>
     <row r="5" spans="1:12" ht="114" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
@@ -720,20 +803,16 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
         <v>16</v>
       </c>
@@ -741,6 +820,142 @@
         <v>17</v>
       </c>
       <c r="L5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="114" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="114" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="114" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="114" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se hacen ajustes de código y documento en varias vistas
</commit_message>
<xml_diff>
--- a/docs/test-cases/contenidoClasesNegocio.xlsx
+++ b/docs/test-cases/contenidoClasesNegocio.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
   <si>
     <t>ID Caso</t>
   </si>
@@ -69,9 +69,6 @@
   </si>
   <si>
     <t>N/A</t>
-  </si>
-  <si>
-    <t>La vista Autodiagnóstico se cargó sin errores</t>
   </si>
   <si>
     <t>OK</t>
@@ -217,6 +214,18 @@
 3.Clic en botón "Seleccionar"
 4.Clic en botón "Página siguiente"
 </t>
+  </si>
+  <si>
+    <t>El sistema permite seleccionar la entidad y mostrar correctamente la vista (Modelos)</t>
+  </si>
+  <si>
+    <t>la vista (modelos) se visualiza correctamente</t>
+  </si>
+  <si>
+    <t>La vista Contenido clases de negocio se cargó sin errores</t>
+  </si>
+  <si>
+    <t>El sistema la creacion de un modelo correctamente</t>
   </si>
 </sst>
 </file>
@@ -626,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -685,10 +694,10 @@
     </row>
     <row r="2" spans="1:12" ht="114" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>12</v>
@@ -697,25 +706,25 @@
         <v>13</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>14</v>
@@ -723,10 +732,10 @@
     </row>
     <row r="3" spans="1:12" ht="114" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
@@ -735,32 +744,36 @@
         <v>13</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="216.75" customHeight="1">
+      <c r="A4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="114" customHeight="1">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>12</v>
@@ -769,21 +782,23 @@
         <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>14</v>
@@ -791,10 +806,10 @@
     </row>
     <row r="5" spans="1:12" ht="114" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>12</v>
@@ -803,10 +818,10 @@
         <v>13</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
@@ -814,10 +829,10 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>14</v>
@@ -825,10 +840,10 @@
     </row>
     <row r="6" spans="1:12" ht="114" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -837,10 +852,10 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
@@ -848,10 +863,10 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>14</v>
@@ -859,10 +874,10 @@
     </row>
     <row r="7" spans="1:12" ht="114" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -871,10 +886,10 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
@@ -882,10 +897,10 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>14</v>
@@ -893,10 +908,10 @@
     </row>
     <row r="8" spans="1:12" ht="114" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
@@ -905,10 +920,10 @@
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
@@ -916,10 +931,10 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>14</v>
@@ -927,10 +942,10 @@
     </row>
     <row r="9" spans="1:12" ht="114" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
@@ -939,10 +954,10 @@
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
@@ -950,10 +965,10 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
se realiza ajustes en código, documento y diagrama en unas vistas
</commit_message>
<xml_diff>
--- a/docs/test-cases/contenidoClasesNegocio.xlsx
+++ b/docs/test-cases/contenidoClasesNegocio.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="contenidoClasesNegocio" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
   <si>
     <t>ID Caso</t>
   </si>
@@ -142,9 +142,111 @@
     <t>Haber seleccionado la entidad modelos opcion editar</t>
   </si>
   <si>
-    <t xml:space="preserve">1.Clic en el botón de la tabla (picklist)
-2.Seleccionar la entidad con ALIAS "Modelos"
-3.Clic en el botón "Seleccionar"
+    <t>CP_CONCLNEG_005</t>
+  </si>
+  <si>
+    <t>Haber seleccionado la entidad modelos opcion eliminar</t>
+  </si>
+  <si>
+    <t>1.Buscar el modelo "TEST EDITAR"
+2.Seleccionar registro con mayor ID
+3.Clic en botón "Eliminar"
+4.Confirmar eliminación en modal.</t>
+  </si>
+  <si>
+    <t>Eliminar modelo</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_006</t>
+  </si>
+  <si>
+    <t>Refrescar vista</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(modelo).</t>
+  </si>
+  <si>
+    <t>1.Clic en el boton refrescar</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_007</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado el botón generar reporte xls</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
+2.Clic en opción 'Exportar todos los registros'
+</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_008</t>
+  </si>
+  <si>
+    <t>Generar reporte xls (opcion exportar todos los registros)</t>
+  </si>
+  <si>
+    <t>Validar funcionamiento del paginador en la vista(Entidad planes comerciales)</t>
+  </si>
+  <si>
+    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(planes comerciales).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
+2.Seleccionar la entidad con ID 135 ("Valores de planes")
+3.Clic en botón "Seleccionar"
+4.Clic en botón "Página siguiente"
+</t>
+  </si>
+  <si>
+    <t>El sistema permite seleccionar la entidad y mostrar correctamente la vista (Modelos)</t>
+  </si>
+  <si>
+    <t>la vista (modelos) se visualiza correctamente</t>
+  </si>
+  <si>
+    <t>La vista Contenido clases de negocio se cargó sin errores</t>
+  </si>
+  <si>
+    <t>El sistema debe realizar la creacion de un modelo correctamente</t>
+  </si>
+  <si>
+    <t>Se crea el modelo correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe realizar la edicion de un modelo correctamente</t>
+  </si>
+  <si>
+    <t>Se edita el modelo correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe realizar la eliminacion de un modelo correctamente</t>
+  </si>
+  <si>
+    <t>Se elimina el modelo correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe refrescar la vista</t>
+  </si>
+  <si>
+    <t>Se refresca la vista correctamente</t>
+  </si>
+  <si>
+    <t>El sistema debe generar el reporte correctamente</t>
+  </si>
+  <si>
+    <t>Se genera el reporte correctamentente</t>
+  </si>
+  <si>
+    <t>El sistema debe navegar por el paginador correctamente</t>
+  </si>
+  <si>
+    <t>Se navega por el paginador correctamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en la barra de búsqueda
+2.Digitar "TEST CREAR" y presionar Enter
+3.Seleccionar registro con ID mayor y validar nombre
 4.Clic en botón Editar.
 5.Clic en el botón del campo "Fabricante" (modo edición)
 6.Seleccionar fabricante con ID 2 (FIBERHOME)
@@ -159,73 +261,56 @@
 </t>
   </si>
   <si>
-    <t>CP_CONCLNEG_005</t>
-  </si>
-  <si>
-    <t>Haber seleccionado la entidad modelos opcion eliminar</t>
-  </si>
-  <si>
-    <t>1.Buscar el modelo "TEST EDITAR"
-2.Seleccionar registro con mayor ID
-3.Clic en botón "Eliminar"
-4.Confirmar eliminación en modal.</t>
-  </si>
-  <si>
-    <t>Eliminar modelo</t>
-  </si>
-  <si>
-    <t>CP_CONCLNEG_006</t>
-  </si>
-  <si>
-    <t>Refrescar vista</t>
-  </si>
-  <si>
-    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(modelo).</t>
-  </si>
-  <si>
-    <t>1.Clic en el boton refrescar</t>
-  </si>
-  <si>
-    <t>CP_CONCLNEG_007</t>
-  </si>
-  <si>
-    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado el botón generar reporte xls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
-2.Clic en opción 'Exportar todos los registros'
+    <t>CP_CONCLNEG_009</t>
+  </si>
+  <si>
+    <t>Filtrar (entidad valores de planes)</t>
+  </si>
+  <si>
+    <t>1.Seleccionar el primer registro de la tabla y capturar datos
+2.Clic en botón "Filtrar"
+3.Llenar modal con datos capturados
+4.Clic en botón "SOCIALSTRATUMID"
+5.Seleccionar el primer registro de la tabla
+6.Clic en botón "Seleccionar" del modal
+7.Clic en botón "MUNICIPALITYID"
+8.Buscar "ESPINAL" en la barra de búsqueda del modal MUNICIPALITYID
+9.Seleccionar resultado de búsqueda en modal MUNICIPALITYID
+10.Clic en botón "Seleccionar" del modal MUNICIPALITYID
+11.Scroll hasta el final y clic en botón "ID PLAN COMERCIAL"
+12.Seleccionar el primer registro del modal "ID PLAN COMERCIAL"
+13.Clic en botón "Seleccionar" del modal ID PLAN COMERCIAL
+14.Clic en botón "Filtrar" del modal cls_commercialplanvalue
+15.</t>
+  </si>
+  <si>
+    <t>El sistema debe filtrar
+el plan comercial deacuerdo
+a la informacion diligenciada</t>
+  </si>
+  <si>
+    <t>FALLA</t>
+  </si>
+  <si>
+    <t>el modal no realiza el filtro con éxito</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón "Carga masiva de objetos"
+2.Clic en botón "Descargar plantilla"
+3.Clic en botón "Cancelar" del modal
 </t>
   </si>
   <si>
-    <t>CP_CONCLNEG_008</t>
-  </si>
-  <si>
-    <t>Generar reporte xls (opcion exportar todos los registros)</t>
-  </si>
-  <si>
-    <t>Validar funcionamiento del paginador en la vista(Entidad planes comerciales)</t>
-  </si>
-  <si>
-    <t>El usuario debe haber accedido a la vista de Contenido clases de negocio y seleccionado una entidad(planes comerciales).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Clic en botón que abre el modal de entidades
-2.Seleccionar la entidad con ID 135 ("Valores de planes")
-3.Clic en botón "Seleccionar"
-4.Clic en botón "Página siguiente"
-</t>
-  </si>
-  <si>
-    <t>El sistema permite seleccionar la entidad y mostrar correctamente la vista (Modelos)</t>
-  </si>
-  <si>
-    <t>la vista (modelos) se visualiza correctamente</t>
-  </si>
-  <si>
-    <t>La vista Contenido clases de negocio se cargó sin errores</t>
-  </si>
-  <si>
-    <t>El sistema la creacion de un modelo correctamente</t>
+    <t>Validar funcionamiento carga masiva de objetos opcion descargar plantilla (entidad valores de planes)</t>
+  </si>
+  <si>
+    <t>El sistema debe abrir el modal de carga masiva y descargar la plantailla correctamente</t>
+  </si>
+  <si>
+    <t>el modal se abrió correctamete y se descarga la planta satisfactoriamente</t>
   </si>
 </sst>
 </file>
@@ -633,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -718,7 +803,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>15</v>
@@ -753,10 +838,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>15</v>
@@ -791,9 +876,11 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
@@ -821,13 +908,17 @@
         <v>32</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>15</v>
       </c>
@@ -840,10 +931,10 @@
     </row>
     <row r="6" spans="1:12" ht="114" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -852,16 +943,20 @@
         <v>13</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>15</v>
       </c>
@@ -874,10 +969,10 @@
     </row>
     <row r="7" spans="1:12" ht="114" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>12</v>
@@ -886,16 +981,20 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
@@ -908,10 +1007,10 @@
     </row>
     <row r="8" spans="1:12" ht="114" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
@@ -920,16 +1019,20 @@
         <v>13</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>61</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
@@ -942,10 +1045,10 @@
     </row>
     <row r="9" spans="1:12" ht="114" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>12</v>
@@ -954,16 +1057,20 @@
         <v>13</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>49</v>
-      </c>
       <c r="G9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>15</v>
       </c>
@@ -971,6 +1078,82 @@
         <v>16</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="114" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="114" customHeight="1">
+      <c r="A11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se realiza nuevamente ajustes en código, excel y diagramas
</commit_message>
<xml_diff>
--- a/docs/test-cases/contenidoClasesNegocio.xlsx
+++ b/docs/test-cases/contenidoClasesNegocio.xlsx
@@ -267,7 +267,36 @@
     <t>Filtrar (entidad valores de planes)</t>
   </si>
   <si>
-    <t>1.Seleccionar el primer registro de la tabla y capturar datos
+    <t>El sistema debe filtrar
+el plan comercial deacuerdo
+a la informacion diligenciada</t>
+  </si>
+  <si>
+    <t>FALLA</t>
+  </si>
+  <si>
+    <t>el modal no realiza el filtro con éxito</t>
+  </si>
+  <si>
+    <t>CP_CONCLNEG_010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Clic en botón "Carga masiva de objetos"
+2.Clic en botón "Descargar plantilla"
+3.Clic en botón "Cancelar" del modal
+</t>
+  </si>
+  <si>
+    <t>Validar funcionamiento carga masiva de objetos opcion descargar plantilla (entidad valores de planes)</t>
+  </si>
+  <si>
+    <t>El sistema debe abrir el modal de carga masiva y descargar la plantailla correctamente</t>
+  </si>
+  <si>
+    <t>el modal se abrió correctamete y se descarga la planta satisfactoriamente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Seleccionar el primer registro de la tabla y capturar datos
 2.Clic en botón "Filtrar"
 3.Llenar modal con datos capturados
 4.Clic en botón "SOCIALSTRATUMID"
@@ -281,36 +310,7 @@
 12.Seleccionar el primer registro del modal "ID PLAN COMERCIAL"
 13.Clic en botón "Seleccionar" del modal ID PLAN COMERCIAL
 14.Clic en botón "Filtrar" del modal cls_commercialplanvalue
-15.</t>
-  </si>
-  <si>
-    <t>El sistema debe filtrar
-el plan comercial deacuerdo
-a la informacion diligenciada</t>
-  </si>
-  <si>
-    <t>FALLA</t>
-  </si>
-  <si>
-    <t>el modal no realiza el filtro con éxito</t>
-  </si>
-  <si>
-    <t>CP_CONCLNEG_010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Clic en botón "Carga masiva de objetos"
-2.Clic en botón "Descargar plantilla"
-3.Clic en botón "Cancelar" del modal
 </t>
-  </si>
-  <si>
-    <t>Validar funcionamiento carga masiva de objetos opcion descargar plantilla (entidad valores de planes)</t>
-  </si>
-  <si>
-    <t>El sistema debe abrir el modal de carga masiva y descargar la plantailla correctamente</t>
-  </si>
-  <si>
-    <t>el modal se abrió correctamete y se descarga la planta satisfactoriamente</t>
   </si>
 </sst>
 </file>
@@ -720,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1098,19 +1098,19 @@
         <v>47</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>69</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>16</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="11" spans="1:12" ht="114" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>12</v>
@@ -1136,16 +1136,16 @@
         <v>47</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>15</v>

</xml_diff>